<commit_message>
Updated concise report and excel diagram
</commit_message>
<xml_diff>
--- a/Excel diagram/diagram.xlsx
+++ b/Excel diagram/diagram.xlsx
@@ -911,11 +911,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112408576"/>
-        <c:axId val="72837376"/>
+        <c:axId val="121845760"/>
+        <c:axId val="82274560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112408576"/>
+        <c:axId val="121845760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72837376"/>
+        <c:crossAx val="82274560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,8 +933,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72837376"/>
+        <c:axId val="82274560"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -944,7 +945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112408576"/>
+        <c:crossAx val="121845760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -956,6 +957,793 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2500000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0800000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9500000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9800000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6699999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5799999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9199999999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.9909999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.238E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4610000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3449999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3419999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.379E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3780000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4790000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.3529999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2763999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0038999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7619999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5340000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.3329999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.424E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.522E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8219999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.13406799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0560000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9354E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7694999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6808E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6595999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1377E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1326999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3164000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.52110400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.199992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15764500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.152922</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.148893</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14833399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2758999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2847000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0013999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="2">
+                  <c:v>0.62792800000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60643800000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59053299999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59629100000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33798899999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32814399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.35824899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>2.4254349999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3632469999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3889550000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.346576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3096300000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.434841</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>#0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="55400448"/>
+        <c:axId val="135260992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="55400448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="135260992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="135260992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55400448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -993,6 +1781,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1290,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>